<commit_message>
Description list and text formmatting
</commit_message>
<xml_diff>
--- a/2024FEB_B3.xlsx
+++ b/2024FEB_B3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>S.N.</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>HTML Lists : ordered and unordered lists with attributes</t>
+  </si>
+  <si>
+    <t>Description list and text formatting in HTML</t>
+  </si>
+  <si>
+    <t>Saturday: Hoiliday</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -143,10 +149,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -483,7 +489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -494,7 +500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -505,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -516,7 +522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -527,25 +533,29 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="8">
         <v>45338</v>
       </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="C7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="8">
         <v>45339</v>
       </c>
-      <c r="C8" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="C8" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -554,7 +564,7 @@
       </c>
       <c r="C9" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -563,7 +573,7 @@
       </c>
       <c r="C10" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -572,7 +582,7 @@
       </c>
       <c r="C11" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -581,7 +591,7 @@
       </c>
       <c r="C12" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -590,7 +600,7 @@
       </c>
       <c r="C13" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Text properties and tables in HTML
</commit_message>
<xml_diff>
--- a/2024FEB_B3.xlsx
+++ b/2024FEB_B3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>S.N.</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Saturday: Hoiliday</t>
+  </si>
+  <si>
+    <t>Text formatting and tables</t>
   </si>
 </sst>
 </file>
@@ -562,7 +565,9 @@
       <c r="B9" s="8">
         <v>45340</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7">

</xml_diff>

<commit_message>
Class started by Bhatta sir
</commit_message>
<xml_diff>
--- a/2024FEB_B3.xlsx
+++ b/2024FEB_B3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>S.N.</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>Text formatting and tables</t>
+  </si>
+  <si>
+    <t>Prajatantra diwas</t>
+  </si>
+  <si>
+    <t>Class by bhatta sir</t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,9 @@
       <c r="B10" s="8">
         <v>45341</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="7">
@@ -585,7 +593,9 @@
       <c r="B11" s="8">
         <v>45342</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="7">

</xml_diff>

<commit_message>
Padding Form and Empty and Non Empty elements
</commit_message>
<xml_diff>
--- a/2024FEB_B3.xlsx
+++ b/2024FEB_B3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>S.N.</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Holiday</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>HTML Table : rowspan, colspan, HTML External Links</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>Phrase elements, margin</t>
+  </si>
+  <si>
+    <t>Empty and Non Empty elements, Padding, HTML  Forms</t>
   </si>
 </sst>
 </file>
@@ -177,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -204,9 +204,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -526,9 +523,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="55.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="28.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="55.57642857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -701,9 +698,7 @@
       <c r="B16" s="8">
         <v>45347</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="C16" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="7">
@@ -712,9 +707,7 @@
       <c r="B17" s="8">
         <v>45348</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="C17" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="7">
@@ -769,7 +762,7 @@
         <v>45354</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
@@ -942,7 +935,7 @@
         <v>45373</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
@@ -953,7 +946,7 @@
         <v>45374</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
@@ -964,7 +957,7 @@
         <v>45375</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
@@ -975,7 +968,7 @@
         <v>45376</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
@@ -985,7 +978,9 @@
       <c r="B46" s="8">
         <v>45377</v>
       </c>
-      <c r="C46" s="9"/>
+      <c r="C46" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="7">

</xml_diff>

<commit_message>
Footer block and Navvigation
</commit_message>
<xml_diff>
--- a/2024FEB_B3.xlsx
+++ b/2024FEB_B3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>S.N.</t>
   </si>
@@ -61,6 +61,9 @@
     <t>Holiday</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>HTML Table : rowspan, colspan, HTML External Links</t>
   </si>
   <si>
@@ -86,6 +89,12 @@
   </si>
   <si>
     <t>HTML Fixed Layout</t>
+  </si>
+  <si>
+    <t>Message box Img and Department block</t>
+  </si>
+  <si>
+    <t>Footer and Navigation</t>
   </si>
 </sst>
 </file>
@@ -186,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -213,6 +222,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -532,9 +544,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="55.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="28.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="55.57642857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -707,7 +719,9 @@
       <c r="B16" s="8">
         <v>45347</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="7">
@@ -716,7 +730,9 @@
       <c r="B17" s="8">
         <v>45348</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="7">
@@ -771,7 +787,7 @@
         <v>45354</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
@@ -944,7 +960,7 @@
         <v>45373</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
@@ -955,7 +971,7 @@
         <v>45374</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
@@ -966,7 +982,7 @@
         <v>45375</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
@@ -977,7 +993,7 @@
         <v>45376</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
@@ -988,7 +1004,7 @@
         <v>45377</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
@@ -999,7 +1015,7 @@
         <v>45378</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
@@ -1010,7 +1026,7 @@
         <v>45379</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
@@ -1021,7 +1037,7 @@
         <v>45380</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
@@ -1040,7 +1056,9 @@
       <c r="B51" s="8">
         <v>45382</v>
       </c>
-      <c r="C51" s="9"/>
+      <c r="C51" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="7">
@@ -1049,7 +1067,9 @@
       <c r="B52" s="8">
         <v>45383</v>
       </c>
-      <c r="C52" s="9"/>
+      <c r="C52" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="7">

</xml_diff>

<commit_message>
HTML multimedia contents and border properties
</commit_message>
<xml_diff>
--- a/2024FEB_B3.xlsx
+++ b/2024FEB_B3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>S.N.</t>
   </si>
@@ -58,18 +58,18 @@
     <t>No Class : bhatta sir</t>
   </si>
   <si>
-    <t>Holiday</t>
+    <t>Saturday Holiday</t>
   </si>
   <si>
     <t>HTML Table : rowspan, colspan, HTML External Links</t>
   </si>
   <si>
+    <t>Bhatta Sir</t>
+  </si>
+  <si>
     <t>Margin, Padding, Project Name Collection</t>
   </si>
   <si>
-    <t>Saturday Holiday</t>
-  </si>
-  <si>
     <t>Fagu Purnima, Holiday</t>
   </si>
   <si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>No class College program</t>
+  </si>
+  <si>
+    <t>Sports Week</t>
+  </si>
+  <si>
+    <t>Ghode Jatra  Holiday</t>
+  </si>
+  <si>
+    <t>Multimedia elements HTML, audio, video, YouTube and Border Properties</t>
   </si>
 </sst>
 </file>
@@ -538,7 +547,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -546,7 +555,7 @@
   <cols>
     <col min="1" max="1" style="10" width="4.576428571428571" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="11" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="55.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="68.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -773,7 +782,9 @@
       <c r="B22" s="8">
         <v>45353</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="7">
@@ -793,7 +804,9 @@
       <c r="B24" s="8">
         <v>45355</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="7">
@@ -802,7 +815,9 @@
       <c r="B25" s="8">
         <v>45356</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="7">
@@ -811,7 +826,9 @@
       <c r="B26" s="8">
         <v>45357</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="7">
@@ -820,7 +837,9 @@
       <c r="B27" s="8">
         <v>45358</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="7">
@@ -829,7 +848,9 @@
       <c r="B28" s="8">
         <v>45359</v>
       </c>
-      <c r="C28" s="9"/>
+      <c r="C28" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="7">
@@ -838,7 +859,9 @@
       <c r="B29" s="8">
         <v>45360</v>
       </c>
-      <c r="C29" s="9"/>
+      <c r="C29" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="7">
@@ -847,7 +870,9 @@
       <c r="B30" s="8">
         <v>45361</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="7">
@@ -856,7 +881,9 @@
       <c r="B31" s="8">
         <v>45362</v>
       </c>
-      <c r="C31" s="9"/>
+      <c r="C31" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="7">
@@ -865,7 +892,9 @@
       <c r="B32" s="8">
         <v>45363</v>
       </c>
-      <c r="C32" s="9"/>
+      <c r="C32" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="7">
@@ -874,7 +903,9 @@
       <c r="B33" s="8">
         <v>45364</v>
       </c>
-      <c r="C33" s="9"/>
+      <c r="C33" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="7">
@@ -883,7 +914,9 @@
       <c r="B34" s="8">
         <v>45365</v>
       </c>
-      <c r="C34" s="9"/>
+      <c r="C34" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="7">
@@ -892,7 +925,9 @@
       <c r="B35" s="8">
         <v>45366</v>
       </c>
-      <c r="C35" s="9"/>
+      <c r="C35" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="7">
@@ -901,7 +936,9 @@
       <c r="B36" s="8">
         <v>45367</v>
       </c>
-      <c r="C36" s="9"/>
+      <c r="C36" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="7">
@@ -910,7 +947,9 @@
       <c r="B37" s="8">
         <v>45368</v>
       </c>
-      <c r="C37" s="9"/>
+      <c r="C37" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="7">
@@ -919,7 +958,9 @@
       <c r="B38" s="8">
         <v>45369</v>
       </c>
-      <c r="C38" s="9"/>
+      <c r="C38" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="7">
@@ -928,7 +969,9 @@
       <c r="B39" s="8">
         <v>45370</v>
       </c>
-      <c r="C39" s="9"/>
+      <c r="C39" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="7">
@@ -937,7 +980,9 @@
       <c r="B40" s="8">
         <v>45371</v>
       </c>
-      <c r="C40" s="9"/>
+      <c r="C40" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="7">
@@ -946,7 +991,9 @@
       <c r="B41" s="8">
         <v>45372</v>
       </c>
-      <c r="C41" s="9"/>
+      <c r="C41" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="7">
@@ -956,7 +1003,7 @@
         <v>45373</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
@@ -967,7 +1014,7 @@
         <v>45374</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
@@ -1043,7 +1090,9 @@
       <c r="B50" s="8">
         <v>45381</v>
       </c>
-      <c r="C50" s="9"/>
+      <c r="C50" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="7">
@@ -1096,7 +1145,9 @@
       <c r="B55" s="8">
         <v>45386</v>
       </c>
-      <c r="C55" s="9"/>
+      <c r="C55" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="7">
@@ -1105,7 +1156,9 @@
       <c r="B56" s="8">
         <v>45387</v>
       </c>
-      <c r="C56" s="9"/>
+      <c r="C56" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="7">
@@ -1114,7 +1167,9 @@
       <c r="B57" s="8">
         <v>45388</v>
       </c>
-      <c r="C57" s="9"/>
+      <c r="C57" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="7">
@@ -1123,16 +1178,193 @@
       <c r="B58" s="8">
         <v>45389</v>
       </c>
-      <c r="C58" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="20.25">
+      <c r="C58" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="7">
         <v>58</v>
       </c>
       <c r="B59" s="8">
         <v>45390</v>
       </c>
-      <c r="C59" s="9"/>
+      <c r="C59" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+      <c r="A60" s="7">
+        <v>59</v>
+      </c>
+      <c r="B60" s="8">
+        <v>45391</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+      <c r="A61" s="7">
+        <v>60</v>
+      </c>
+      <c r="B61" s="8">
+        <v>45392</v>
+      </c>
+      <c r="C61" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="A62" s="7">
+        <v>61</v>
+      </c>
+      <c r="B62" s="8">
+        <v>45393</v>
+      </c>
+      <c r="C62" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+      <c r="A63" s="7">
+        <v>62</v>
+      </c>
+      <c r="B63" s="8">
+        <v>45394</v>
+      </c>
+      <c r="C63" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+      <c r="A64" s="7">
+        <v>63</v>
+      </c>
+      <c r="B64" s="8">
+        <v>45395</v>
+      </c>
+      <c r="C64" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+      <c r="A65" s="7">
+        <v>64</v>
+      </c>
+      <c r="B65" s="8">
+        <v>45396</v>
+      </c>
+      <c r="C65" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+      <c r="A66" s="7">
+        <v>65</v>
+      </c>
+      <c r="B66" s="8">
+        <v>45397</v>
+      </c>
+      <c r="C66" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+      <c r="A67" s="7">
+        <v>66</v>
+      </c>
+      <c r="B67" s="8">
+        <v>45398</v>
+      </c>
+      <c r="C67" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+      <c r="A68" s="7">
+        <v>67</v>
+      </c>
+      <c r="B68" s="8">
+        <v>45399</v>
+      </c>
+      <c r="C68" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+      <c r="A69" s="7">
+        <v>68</v>
+      </c>
+      <c r="B69" s="8">
+        <v>45400</v>
+      </c>
+      <c r="C69" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+      <c r="A70" s="7">
+        <v>69</v>
+      </c>
+      <c r="B70" s="8">
+        <v>45401</v>
+      </c>
+      <c r="C70" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+      <c r="A71" s="7">
+        <v>70</v>
+      </c>
+      <c r="B71" s="8">
+        <v>45402</v>
+      </c>
+      <c r="C71" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+      <c r="A72" s="7">
+        <v>71</v>
+      </c>
+      <c r="B72" s="8">
+        <v>45403</v>
+      </c>
+      <c r="C72" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+      <c r="A73" s="7">
+        <v>72</v>
+      </c>
+      <c r="B73" s="8">
+        <v>45404</v>
+      </c>
+      <c r="C73" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+      <c r="A74" s="7">
+        <v>73</v>
+      </c>
+      <c r="B74" s="8">
+        <v>45405</v>
+      </c>
+      <c r="C74" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+      <c r="A75" s="7">
+        <v>74</v>
+      </c>
+      <c r="B75" s="8">
+        <v>45406</v>
+      </c>
+      <c r="C75" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+      <c r="A76" s="7">
+        <v>75</v>
+      </c>
+      <c r="B76" s="8">
+        <v>45407</v>
+      </c>
+      <c r="C76" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+      <c r="A77" s="7">
+        <v>76</v>
+      </c>
+      <c r="B77" s="8">
+        <v>45408</v>
+      </c>
+      <c r="C77" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+      <c r="A78" s="7">
+        <v>77</v>
+      </c>
+      <c r="B78" s="8">
+        <v>45409</v>
+      </c>
+      <c r="C78" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CSS text and table properties
</commit_message>
<xml_diff>
--- a/2024FEB_B3.xlsx
+++ b/2024FEB_B3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>S.N.</t>
   </si>
@@ -107,6 +107,24 @@
   </si>
   <si>
     <t>Multimedia elements HTML, audio, video, YouTube and Border Properties</t>
+  </si>
+  <si>
+    <t>ED Holiday</t>
+  </si>
+  <si>
+    <t>Website landing page assignment</t>
+  </si>
+  <si>
+    <t>Landing Page</t>
+  </si>
+  <si>
+    <t>Inernal Links HTML and Character Entities</t>
+  </si>
+  <si>
+    <t>CSS Table and Text Properties</t>
+  </si>
+  <si>
+    <t>Ram Nawami Holiday</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1211,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -1204,79 +1222,95 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="7">
         <v>60</v>
       </c>
       <c r="B61" s="8">
         <v>45392</v>
       </c>
-      <c r="C61" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="C61" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="7">
         <v>61</v>
       </c>
       <c r="B62" s="8">
         <v>45393</v>
       </c>
-      <c r="C62" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+      <c r="C62" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="7">
         <v>62</v>
       </c>
       <c r="B63" s="8">
         <v>45394</v>
       </c>
-      <c r="C63" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+      <c r="C63" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="7">
         <v>63</v>
       </c>
       <c r="B64" s="8">
         <v>45395</v>
       </c>
-      <c r="C64" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+      <c r="C64" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="7">
         <v>64</v>
       </c>
       <c r="B65" s="8">
         <v>45396</v>
       </c>
-      <c r="C65" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+      <c r="C65" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="7">
         <v>65</v>
       </c>
       <c r="B66" s="8">
         <v>45397</v>
       </c>
-      <c r="C66" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+      <c r="C66" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="7">
         <v>66</v>
       </c>
       <c r="B67" s="8">
         <v>45398</v>
       </c>
-      <c r="C67" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+      <c r="C67" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="7">
         <v>67</v>
       </c>
       <c r="B68" s="8">
         <v>45399</v>
       </c>
-      <c r="C68" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+      <c r="C68" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -1285,7 +1319,7 @@
       </c>
       <c r="C69" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -1294,7 +1328,7 @@
       </c>
       <c r="C70" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="7">
         <v>70</v>
       </c>
@@ -1303,7 +1337,7 @@
       </c>
       <c r="C71" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="7">
         <v>71</v>
       </c>
@@ -1312,7 +1346,7 @@
       </c>
       <c r="C72" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="7">
         <v>72</v>
       </c>
@@ -1321,7 +1355,7 @@
       </c>
       <c r="C73" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -1330,7 +1364,7 @@
       </c>
       <c r="C74" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="7">
         <v>74</v>
       </c>
@@ -1339,7 +1373,7 @@
       </c>
       <c r="C75" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -1348,7 +1382,7 @@
       </c>
       <c r="C76" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="7">
         <v>76</v>
       </c>
@@ -1357,7 +1391,7 @@
       </c>
       <c r="C77" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="20.25">
       <c r="A78" s="7">
         <v>77</v>
       </c>

</xml_diff>